<commit_message>
Implementing Household Visit Fragment and views
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/member_enu_form.xlsx
+++ b/app/src/main/res/raw/member_enu_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11895" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="30720" windowHeight="13512" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -15,8 +15,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>paul</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t>paul:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="Times New Roman"/>
+            <charset val="0"/>
+          </rPr>
+          <t xml:space="preserve">
+The option is readonly, not choosable.
+Only selectable programatically, when selected make the all options read-only
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
   <si>
     <t>group</t>
   </si>
@@ -51,6 +85,9 @@
     <t>readonly</t>
   </si>
   <si>
+    <t>display_condition</t>
+  </si>
+  <si>
     <t>header</t>
   </si>
   <si>
@@ -177,6 +214,9 @@
     <t>3.5. Data do Censo?</t>
   </si>
   <si>
+    <t>collected</t>
+  </si>
+  <si>
     <t>collectedBy</t>
   </si>
   <si>
@@ -201,6 +241,15 @@
     <t>4.2. Data da Visita</t>
   </si>
   <si>
+    <t>modules</t>
+  </si>
+  <si>
+    <t>Access Granted to Modules</t>
+  </si>
+  <si>
+    <t>Acesso permitido ao Módulos</t>
+  </si>
+  <si>
     <t>value</t>
   </si>
   <si>
@@ -222,46 +271,82 @@
     <t>Feminino</t>
   </si>
   <si>
+    <t>HOH</t>
+  </si>
+  <si>
+    <t>Head of Household</t>
+  </si>
+  <si>
+    <t>Chefe do Agregado</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>SPO</t>
+  </si>
+  <si>
     <t>Spouse</t>
   </si>
   <si>
     <t>Esposo/a</t>
   </si>
   <si>
+    <t>SON</t>
+  </si>
+  <si>
     <t>Son/Daughter</t>
   </si>
   <si>
     <t>Filho/Filha</t>
   </si>
   <si>
+    <t>BRO</t>
+  </si>
+  <si>
     <t>Brother/Sister</t>
   </si>
   <si>
     <t>Irmão/Irmã</t>
   </si>
   <si>
+    <t>PAR</t>
+  </si>
+  <si>
     <t>Parent</t>
   </si>
   <si>
     <t>Pai/Mãe</t>
   </si>
   <si>
+    <t>GCH</t>
+  </si>
+  <si>
     <t>Grandchild</t>
   </si>
   <si>
     <t>Neto/a</t>
   </si>
   <si>
+    <t>NOR</t>
+  </si>
+  <si>
     <t>Not Related</t>
   </si>
   <si>
     <t>Sem relação</t>
   </si>
   <si>
+    <t>OTH</t>
+  </si>
+  <si>
     <t>Other Relative</t>
   </si>
   <si>
     <t>Outro parente</t>
+  </si>
+  <si>
+    <t>DNK</t>
   </si>
   <si>
     <t>Don't Know</t>
@@ -293,12 +378,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="26">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -322,6 +407,50 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Arial"/>
@@ -329,10 +458,64 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -344,40 +527,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -389,25 +543,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -421,56 +558,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -482,19 +578,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,31 +698,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,127 +740,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -673,6 +769,60 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -700,47 +850,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -755,173 +869,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -939,6 +1035,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -1257,25 +1359,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="11.1428571428571" customWidth="true"/>
-    <col min="3" max="3" width="14.1428571428571" customWidth="true"/>
-    <col min="4" max="4" width="20.1428571428571" customWidth="true"/>
-    <col min="5" max="5" width="11.7142857142857" customWidth="true"/>
-    <col min="6" max="6" width="12.2857142857143" customWidth="true"/>
+    <col min="2" max="2" width="11.1388888888889" customWidth="true"/>
+    <col min="3" max="3" width="14.1388888888889" customWidth="true"/>
+    <col min="4" max="4" width="20.1388888888889" customWidth="true"/>
+    <col min="5" max="5" width="11.712962962963" customWidth="true"/>
+    <col min="6" max="6" width="12.287037037037" customWidth="true"/>
     <col min="7" max="8" width="41" customWidth="true"/>
-    <col min="9" max="9" width="21.7142857142857" customWidth="true"/>
-    <col min="10" max="10" width="9.28571428571429" customWidth="true"/>
+    <col min="9" max="9" width="21.712962962963" customWidth="true"/>
+    <col min="10" max="10" width="9.28703703703704" customWidth="true"/>
+    <col min="12" max="12" width="16.5740740740741" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1309,24 +1412,27 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="8" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="7"/>
+        <v>16</v>
+      </c>
+      <c r="I2" s="9"/>
       <c r="J2" t="b">
         <v>1</v>
       </c>
@@ -1336,21 +1442,21 @@
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="I3" s="9"/>
       <c r="J3" t="b">
         <v>1</v>
       </c>
@@ -1360,21 +1466,21 @@
     </row>
     <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="7"/>
+        <v>22</v>
+      </c>
+      <c r="I4" s="9"/>
       <c r="J4" t="b">
         <v>1</v>
       </c>
@@ -1384,21 +1490,21 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="7"/>
+        <v>26</v>
+      </c>
+      <c r="I5" s="9"/>
       <c r="J5" t="b">
         <v>1</v>
       </c>
@@ -1408,22 +1514,22 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="7"/>
+        <v>29</v>
+      </c>
+      <c r="I6" s="9"/>
       <c r="J6" t="b">
         <v>1</v>
       </c>
@@ -1433,21 +1539,21 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="7"/>
+        <v>32</v>
+      </c>
+      <c r="I7" s="9"/>
       <c r="J7" t="b">
         <v>1</v>
       </c>
@@ -1457,21 +1563,21 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
-      </c>
-      <c r="I8" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="I8" s="9"/>
       <c r="J8" t="b">
         <v>1</v>
       </c>
@@ -1484,36 +1590,36 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I9" s="7"/>
+        <v>37</v>
+      </c>
+      <c r="I9" s="9"/>
       <c r="J9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="4:10">
       <c r="D10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
-      </c>
-      <c r="I10" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="I10" s="9"/>
       <c r="J10" t="b">
         <v>1</v>
       </c>
@@ -1521,18 +1627,18 @@
     <row r="11" spans="1:10">
       <c r="A11" s="1"/>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
-      </c>
-      <c r="I11" s="7"/>
+        <v>46</v>
+      </c>
+      <c r="I11" s="9"/>
       <c r="J11" t="b">
         <v>1</v>
       </c>
@@ -1540,21 +1646,21 @@
     <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G12" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
-      </c>
-      <c r="I12" s="7"/>
+        <v>50</v>
+      </c>
+      <c r="I12" s="9"/>
       <c r="J12" t="b">
         <v>1</v>
       </c>
@@ -1562,38 +1668,40 @@
     <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H13" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="7"/>
+        <v>53</v>
+      </c>
+      <c r="I13" s="9"/>
       <c r="J13" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D14" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
-      </c>
-      <c r="I14" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="I14" s="9"/>
       <c r="J14" t="b">
         <v>1</v>
       </c>
@@ -1602,20 +1710,22 @@
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D15" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H15" t="s">
-        <v>60</v>
-      </c>
-      <c r="I15" s="7"/>
+        <v>62</v>
+      </c>
+      <c r="I15" s="9"/>
       <c r="J15" t="b">
         <v>1</v>
       </c>
@@ -1623,21 +1733,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="1"/>
-      <c r="I16" s="7"/>
+    <row r="16" spans="1:11">
+      <c r="A16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>64</v>
+      </c>
+      <c r="H16" t="s">
+        <v>65</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="1"/>
-      <c r="I17" s="7"/>
+      <c r="I17" s="9"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1"/>
-      <c r="I18" s="7"/>
+      <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1"/>
-      <c r="I19" s="8"/>
+      <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="1"/>
@@ -1685,26 +1815,27 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="12.5714285714286" customWidth="true"/>
-    <col min="2" max="2" width="12.2857142857143" customWidth="true"/>
-    <col min="3" max="4" width="13.8571428571429" customWidth="true"/>
-    <col min="5" max="5" width="13.1428571428571" customWidth="true"/>
+    <col min="1" max="1" width="12.5740740740741" customWidth="true"/>
+    <col min="2" max="2" width="12.287037037037" customWidth="true"/>
+    <col min="3" max="3" width="18.1388888888889" customWidth="true"/>
+    <col min="4" max="4" width="18.287037037037" customWidth="true"/>
+    <col min="5" max="5" width="13.1388888888889" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1712,152 +1843,173 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>69</v>
+    <row r="4" spans="1:5">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="5">
-        <v>3</v>
+        <v>48</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="5">
-        <v>4</v>
+        <v>48</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="5">
-        <v>5</v>
+        <v>48</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="5">
-        <v>6</v>
+        <v>48</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="5">
-        <v>7</v>
+        <v>48</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>89</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="5">
-        <v>8</v>
+        <v>48</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="5">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>83</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1866,37 +2018,37 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="true"/>
-    <col min="2" max="2" width="20.4285714285714" customWidth="true"/>
-    <col min="3" max="3" width="23.2857142857143" customWidth="true"/>
+    <col min="2" max="2" width="20.4259259259259" customWidth="true"/>
+    <col min="3" max="3" width="23.287037037037" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- Add Member Enumeration registration through Household Visit - Add clear member selection feature to goto Household Mode after Member Mode - Reload fragments after visit
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/member_enu_form.xlsx
+++ b/app/src/main/res/raw/member_enu_form.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="30720" windowHeight="13512" tabRatio="500"/>
+    <workbookView windowWidth="21000" windowHeight="11895" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="columns" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
   <si>
     <t>group</t>
   </si>
@@ -91,10 +91,19 @@
     <t>header</t>
   </si>
   <si>
+    <t>visitCode</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>1.0. Visit Code</t>
+  </si>
+  <si>
+    <t>1.0. Código da Visita</t>
+  </si>
+  <si>
     <t>code</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
   <si>
     <t>1.1. Member Code</t>
@@ -378,9 +387,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
@@ -423,16 +432,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -444,20 +462,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -466,6 +470,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -474,6 +538,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -482,77 +560,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -578,187 +587,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -772,32 +781,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -828,23 +831,25 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -859,155 +864,159 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="4" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1017,7 +1026,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center"/>
@@ -1037,6 +1046,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
@@ -1359,23 +1371,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:K16"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="11.1388888888889" customWidth="true"/>
-    <col min="3" max="3" width="14.1388888888889" customWidth="true"/>
-    <col min="4" max="4" width="20.1388888888889" customWidth="true"/>
-    <col min="5" max="5" width="11.712962962963" customWidth="true"/>
-    <col min="6" max="6" width="12.287037037037" customWidth="true"/>
-    <col min="7" max="8" width="41" customWidth="true"/>
-    <col min="9" max="9" width="21.712962962963" customWidth="true"/>
-    <col min="10" max="10" width="9.28703703703704" customWidth="true"/>
-    <col min="12" max="12" width="16.5740740740741" customWidth="true"/>
+    <col min="2" max="2" customWidth="true" width="11.1428571428571" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.1428571428571" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.1428571428571" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.7142857142857" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.2857142857143" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="41.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.6761904761905" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="21.7142857142857" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="9.28571428571429" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.5714285714286" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1412,33 +1425,37 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
@@ -1456,7 +1473,7 @@
       <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="9"/>
+      <c r="I3" s="10"/>
       <c r="J3" t="b">
         <v>1</v>
       </c>
@@ -1480,7 +1497,7 @@
       <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="10"/>
       <c r="J4" t="b">
         <v>1</v>
       </c>
@@ -1490,21 +1507,21 @@
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="9"/>
+      <c r="I5" s="10"/>
       <c r="J5" t="b">
         <v>1</v>
       </c>
@@ -1514,7 +1531,7 @@
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -1522,14 +1539,13 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="1"/>
       <c r="G6" t="s">
         <v>28</v>
       </c>
       <c r="H6" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="9"/>
+      <c r="I6" s="10"/>
       <c r="J6" t="b">
         <v>1</v>
       </c>
@@ -1539,7 +1555,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
@@ -1547,13 +1563,14 @@
       <c r="E7" t="s">
         <v>14</v>
       </c>
+      <c r="F7" s="1"/>
       <c r="G7" t="s">
         <v>31</v>
       </c>
       <c r="H7" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="9"/>
+      <c r="I7" s="10"/>
       <c r="J7" t="b">
         <v>1</v>
       </c>
@@ -1563,7 +1580,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
         <v>33</v>
@@ -1577,7 +1594,7 @@
       <c r="H8" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="10"/>
       <c r="J8" t="b">
         <v>1</v>
       </c>
@@ -1585,60 +1602,65 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="4:10">
+    <row r="9" spans="1:11">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="9"/>
+        <v>38</v>
+      </c>
+      <c r="I9" s="10"/>
       <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="4:10">
       <c r="D10" t="s">
-        <v>38</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>40</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" s="10"/>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10">
+      <c r="D11" t="s">
         <v>41</v>
       </c>
-      <c r="H10" t="s">
+      <c r="E11" t="s">
         <v>42</v>
       </c>
-      <c r="I10" s="9"/>
-      <c r="J10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="1"/>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>44</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>45</v>
       </c>
-      <c r="H11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="10"/>
       <c r="J11" t="b">
         <v>1</v>
       </c>
@@ -1646,21 +1668,18 @@
     <row r="12" spans="1:10">
       <c r="A12" s="1"/>
       <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>48</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>49</v>
       </c>
-      <c r="H12" t="s">
-        <v>50</v>
-      </c>
-      <c r="I12" s="9"/>
+      <c r="I12" s="10"/>
       <c r="J12" t="b">
         <v>1</v>
       </c>
@@ -1668,10 +1687,13 @@
     <row r="13" spans="1:10">
       <c r="A13" s="1"/>
       <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" t="s">
         <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>44</v>
       </c>
       <c r="G13" t="s">
         <v>52</v>
@@ -1679,53 +1701,48 @@
       <c r="H13" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="10"/>
       <c r="J13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:10">
+      <c r="A14" s="1"/>
+      <c r="D14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" t="s">
         <v>55</v>
       </c>
-      <c r="E14" t="s">
+      <c r="H14" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="1"/>
-      <c r="G14" t="s">
-        <v>57</v>
-      </c>
-      <c r="H14" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="10"/>
       <c r="J14" t="b">
-        <v>1</v>
-      </c>
-      <c r="K14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
         <v>59</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" s="1"/>
+      <c r="G15" t="s">
         <v>60</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>61</v>
       </c>
-      <c r="H15" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="10"/>
       <c r="J15" t="b">
         <v>1</v>
       </c>
@@ -1735,13 +1752,13 @@
     </row>
     <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" t="s">
         <v>63</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
       </c>
       <c r="G16" t="s">
         <v>64</v>
@@ -1749,7 +1766,7 @@
       <c r="H16" t="s">
         <v>65</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="10"/>
       <c r="J16" t="b">
         <v>1</v>
       </c>
@@ -1757,20 +1774,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="1"/>
-      <c r="I17" s="9"/>
+    <row r="17" spans="1:11">
+      <c r="A17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" s="10"/>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="1"/>
-      <c r="I18" s="9"/>
+      <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="1"/>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:9">
       <c r="A20" s="1"/>
+      <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="1"/>
@@ -1804,6 +1842,9 @@
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="1"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="0.7875" bottom="0.7875" header="0.39375" footer="0.39375"/>
@@ -1817,17 +1858,17 @@
   <sheetPr/>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="12.5740740740741" customWidth="true"/>
-    <col min="2" max="2" width="12.287037037037" customWidth="true"/>
-    <col min="3" max="3" width="18.1388888888889" customWidth="true"/>
-    <col min="4" max="4" width="18.287037037037" customWidth="true"/>
-    <col min="5" max="5" width="13.1388888888889" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="12.5714285714286" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.2857142857143" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.1428571428571" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.2857142857143" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.1428571428571" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1835,7 +1876,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -1849,161 +1890,161 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2022,33 +2063,33 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.13888888888889" defaultRowHeight="13.2" outlineLevelRow="1" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="true"/>
-    <col min="2" max="2" width="20.4259259259259" customWidth="true"/>
-    <col min="3" max="3" width="23.287037037037" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.4285714285714" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.2857142857143" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>